<commit_message>
Cambi discussi in riunione riguardo il sorting commesse e il check3 delle ricerche locali
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/insert_inter.xlsx
+++ b/PS-VRP/OUTPUT_TEST/insert_inter.xlsx
@@ -512,7 +512,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251327</v>
+        <v>251550</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -520,10 +520,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>261.625</v>
+        <v>557.046875</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -532,21 +532,21 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-04-10 10:16:00</t>
+          <t>2025-04-10 10:14:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-04-10 10:16:00</t>
+          <t>2025-04-10 10:14:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-04-10 14:37:37</t>
+          <t>2025-04-11 11:31:02</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>16744</v>
+        <v>35651</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -559,18 +559,18 @@
         </is>
       </c>
       <c r="L2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M2" t="n">
+        <v>70</v>
+      </c>
+      <c r="N2" t="n">
         <v>4</v>
-      </c>
-      <c r="M2" t="n">
-        <v>70</v>
-      </c>
-      <c r="N2" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251100</v>
+        <v>250478</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -578,33 +578,33 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>72.828125</v>
+        <v>65.375</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-04-10 14:37:37</t>
+          <t>2025-04-11 11:31:02</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-04-10 14:52:37</t>
+          <t>2025-04-11 11:50:02</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-04-10 14:52:37</t>
+          <t>2025-04-11 11:50:02</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-04-11 08:05:27</t>
+          <t>2025-04-11 12:55:25</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>4661</v>
+        <v>4184</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -617,18 +617,15 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M3" t="n">
         <v>70</v>
-      </c>
-      <c r="N3" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251033</v>
+        <v>250855</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -639,30 +636,30 @@
         <v>19</v>
       </c>
       <c r="D4" t="n">
-        <v>96.03125</v>
+        <v>443.890625</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-04-11 08:05:27</t>
+          <t>2025-04-11 12:55:25</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-04-11 08:24:27</t>
+          <t>2025-04-11 13:14:25</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-04-11 08:24:27</t>
+          <t>2025-04-11 13:14:25</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-04-11 10:00:29</t>
+          <t>2025-04-14 12:38:18</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>6146</v>
+        <v>28409</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -675,18 +672,15 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M4" t="n">
         <v>70</v>
-      </c>
-      <c r="N4" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>245413</v>
+        <v>250637</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -694,33 +688,33 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D5" t="n">
-        <v>78.125</v>
+        <v>585.578125</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-11 10:00:29</t>
+          <t>2025-04-14 12:38:18</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-04-11 10:17:29</t>
+          <t>2025-04-14 12:59:18</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-04-11 10:17:29</t>
+          <t>2025-04-14 12:59:18</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-04-11 11:35:36</t>
+          <t>2025-04-15 14:44:53</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>5000</v>
+        <v>37477</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -729,22 +723,19 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
-      </c>
-      <c r="N5" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>244023</v>
+        <v>250780</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -752,33 +743,33 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6" t="n">
-        <v>15.578125</v>
+        <v>408.3125</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-04-11 11:35:36</t>
+          <t>2025-04-15 14:44:53</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-04-11 11:56:36</t>
+          <t>2025-04-16 07:07:53</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-04-11 11:56:36</t>
+          <t>2025-04-16 07:07:53</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-04-11 12:12:11</t>
+          <t>2025-04-16 13:56:12</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>997</v>
+        <v>26132</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -787,22 +778,22 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
+        <v>10</v>
+      </c>
+      <c r="M6" t="n">
+        <v>70</v>
+      </c>
+      <c r="N6" t="n">
         <v>6</v>
-      </c>
-      <c r="M6" t="n">
-        <v>70</v>
-      </c>
-      <c r="N6" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251134</v>
+        <v>251150</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -810,33 +801,33 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" t="n">
-        <v>68.703125</v>
+        <v>709.375</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-04-11 12:12:11</t>
+          <t>2025-04-16 13:56:12</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-04-11 12:27:11</t>
+          <t>2025-04-16 14:13:12</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-04-11 12:27:11</t>
+          <t>2025-04-16 14:13:12</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-04-11 13:35:53</t>
+          <t>2025-04-18 10:02:34</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>4397</v>
+        <v>45400</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -845,11 +836,11 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
@@ -857,41 +848,41 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>250856</v>
+        <v>243335</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>236.75</v>
+        <v>464.8450704225352</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-04-11 13:35:53</t>
+          <t>2025-04-10 14:19:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-04-11 13:56:53</t>
+          <t>2025-04-10 14:36:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-04-11 13:56:53</t>
+          <t>2025-04-10 14:36:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-04-14 09:53:38</t>
+          <t>2025-04-11 14:20:50</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>15152</v>
+        <v>33004</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -900,53 +891,56 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M8" t="n">
-        <v>70</v>
+        <v>152</v>
+      </c>
+      <c r="N8" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251097</v>
+        <v>251088</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D9" t="n">
-        <v>271.265625</v>
+        <v>87.11267605633803</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-04-14 09:53:38</t>
+          <t>2025-04-11 14:20:50</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-04-14 10:08:38</t>
+          <t>2025-04-11 14:52:50</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-04-14 10:08:38</t>
+          <t>2025-04-11 14:52:50</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-04-14 14:39:54</t>
+          <t>2025-04-14 08:19:57</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>17361</v>
+        <v>6185</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -965,46 +959,46 @@
         <v>70</v>
       </c>
       <c r="N9" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251522</v>
+        <v>235572</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D10" t="n">
-        <v>610.953125</v>
+        <v>140.2535211267606</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-04-14 14:39:54</t>
+          <t>2025-04-14 08:19:57</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-04-14 14:56:54</t>
+          <t>2025-04-14 08:38:57</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-04-14 14:56:54</t>
+          <t>2025-04-14 08:38:57</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-04-16 09:07:51</t>
+          <t>2025-04-14 10:59:12</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>39101</v>
+        <v>9958</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1013,11 +1007,11 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
@@ -1028,41 +1022,41 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251346</v>
+        <v>251015</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D11" t="n">
-        <v>60.296875</v>
+        <v>179.0422535211268</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-04-16 09:07:51</t>
+          <t>2025-04-14 10:59:12</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-04-16 09:34:51</t>
+          <t>2025-04-14 11:18:12</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-04-16 09:34:51</t>
+          <t>2025-04-14 11:18:12</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-04-16 10:35:09</t>
+          <t>2025-04-14 14:17:15</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>3859</v>
+        <v>12712</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1075,52 +1069,49 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M11" t="n">
         <v>70</v>
-      </c>
-      <c r="N11" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>250866</v>
+        <v>250307</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" t="n">
-        <v>79.9375</v>
+        <v>131.8169014084507</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-04-16 10:35:09</t>
+          <t>2025-04-14 14:17:15</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-04-16 10:54:09</t>
+          <t>2025-04-14 14:34:15</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-04-16 10:54:09</t>
+          <t>2025-04-14 14:34:15</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-04-16 12:14:05</t>
+          <t>2025-04-15 08:46:04</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>5116</v>
+        <v>9359</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1133,52 +1124,49 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M12" t="n">
         <v>70</v>
-      </c>
-      <c r="N12" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>250479</v>
+        <v>251235</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D13" t="n">
-        <v>257.296875</v>
+        <v>80.83098591549296</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-04-16 12:14:05</t>
+          <t>2025-04-15 08:46:04</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-04-16 12:31:05</t>
+          <t>2025-04-15 09:07:04</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-04-16 12:31:05</t>
+          <t>2025-04-15 09:07:04</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-04-17 08:48:23</t>
+          <t>2025-04-15 10:27:54</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>16467</v>
+        <v>5739</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1187,7 +1175,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L13" t="n">
@@ -1199,41 +1187,41 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251204</v>
+        <v>250635</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D14" t="n">
-        <v>119.734375</v>
+        <v>131.9577464788732</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-04-17 08:48:23</t>
+          <t>2025-04-15 10:27:54</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-04-17 09:09:23</t>
+          <t>2025-04-15 10:44:54</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-04-17 09:09:23</t>
+          <t>2025-04-15 10:44:54</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-04-17 11:09:07</t>
+          <t>2025-04-15 12:56:51</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>7663</v>
+        <v>9369</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1242,56 +1230,53 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M14" t="n">
         <v>70</v>
-      </c>
-      <c r="N14" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>245623</v>
+        <v>251402</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>412.796875</v>
+        <v>139.5774647887324</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-04-17 11:09:07</t>
+          <t>2025-04-15 12:56:51</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-04-17 11:39:07</t>
+          <t>2025-04-15 13:13:51</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-04-17 11:39:07</t>
+          <t>2025-04-15 13:13:51</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-04-18 10:31:55</t>
+          <t>2025-04-16 07:33:26</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>26419</v>
+        <v>9910</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1300,53 +1285,56 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M15" t="n">
-        <v>152</v>
+        <v>70</v>
+      </c>
+      <c r="N15" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251094</v>
+        <v>251097</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>19</v>
+        <v>34.5</v>
       </c>
       <c r="D16" t="n">
-        <v>210.890625</v>
+        <v>315.6545454545454</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-04-18 10:31:55</t>
+          <t>2025-04-10 10:41:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-04-18 10:50:55</t>
+          <t>2025-04-10 11:15:30</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-04-18 10:50:55</t>
+          <t>2025-04-10 11:15:30</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-04-18 14:21:48</t>
+          <t>2025-04-11 08:31:09</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>13497</v>
+        <v>17361</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1355,56 +1343,56 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N16" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>243569</v>
+        <v>251281</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>32</v>
+        <v>38.5</v>
       </c>
       <c r="D17" t="n">
-        <v>40.640625</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-04-18 14:21:48</t>
+          <t>2025-04-11 08:31:09</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-04-18 14:53:48</t>
+          <t>2025-04-11 09:09:39</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-04-18 14:53:48</t>
+          <t>2025-04-11 09:09:39</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-04-21 07:34:27</t>
+          <t>2025-04-11 14:06:44</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>2601</v>
+        <v>16340</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1413,56 +1401,56 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M17" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251129</v>
+        <v>251280</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>19</v>
+        <v>30.5</v>
       </c>
       <c r="D18" t="n">
-        <v>112.390625</v>
+        <v>346.6</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-04-21 07:34:27</t>
+          <t>2025-04-11 14:06:44</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-04-21 07:53:27</t>
+          <t>2025-04-11 14:37:14</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-04-21 07:53:27</t>
+          <t>2025-04-11 14:37:14</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-04-21 09:45:50</t>
+          <t>2025-04-14 12:23:50</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>7193</v>
+        <v>19063</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1471,56 +1459,56 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M18" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N18" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251519</v>
+        <v>251442</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>36</v>
+        <v>30.5</v>
       </c>
       <c r="D19" t="n">
-        <v>205.859375</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-04-21 09:45:50</t>
+          <t>2025-04-14 12:23:50</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-04-21 10:21:50</t>
+          <t>2025-04-14 12:54:20</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-04-21 10:21:50</t>
+          <t>2025-04-14 12:54:20</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-04-21 13:47:42</t>
+          <t>2025-04-15 09:51:26</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>13175</v>
+        <v>16340</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1529,53 +1517,56 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L19" t="n">
+        <v>7</v>
+      </c>
+      <c r="M19" t="n">
+        <v>70</v>
+      </c>
+      <c r="N19" t="n">
         <v>2</v>
-      </c>
-      <c r="M19" t="n">
-        <v>70</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>250966</v>
+        <v>251285</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="D20" t="n">
-        <v>135.640625</v>
+        <v>950.344262295082</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-04-21 13:47:42</t>
+          <t>2025-04-10 14:33:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-04-21 14:04:42</t>
+          <t>2025-04-11 08:33:00</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-04-21 14:04:42</t>
+          <t>2025-04-11 08:33:00</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-04-22 08:20:20</t>
+          <t>2025-04-15 08:23:20</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>8681</v>
+        <v>57971</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1588,7 +1579,7 @@
         </is>
       </c>
       <c r="L20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
         <v>70</v>
@@ -1596,41 +1587,41 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251088</v>
+        <v>243569</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D21" t="n">
-        <v>96.640625</v>
+        <v>36.63380281690141</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-04-22 08:20:20</t>
+          <t>2025-04-10 10:00:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-04-22 08:35:20</t>
+          <t>2025-04-10 10:48:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-04-22 08:35:20</t>
+          <t>2025-04-10 10:48:00</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-04-22 10:11:59</t>
+          <t>2025-04-10 11:24:38</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>6185</v>
+        <v>2601</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1639,14 +1630,14 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
         <v>3</v>
       </c>
       <c r="M21" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N21" t="n">
         <v>3</v>
@@ -1654,41 +1645,41 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>235572</v>
+        <v>250497</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" t="n">
-        <v>155.59375</v>
+        <v>267.4647887323944</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-04-22 10:11:59</t>
+          <t>2025-04-10 11:24:38</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-04-22 10:30:59</t>
+          <t>2025-04-10 11:41:38</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-04-22 10:30:59</t>
+          <t>2025-04-10 11:41:38</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-04-22 13:06:34</t>
+          <t>2025-04-11 08:09:05</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>9958</v>
+        <v>18990</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1697,56 +1688,53 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M22" t="n">
-        <v>70</v>
-      </c>
-      <c r="N22" t="n">
-        <v>3</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251015</v>
+        <v>245089</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D23" t="n">
-        <v>198.625</v>
+        <v>1727.676056338028</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-04-22 13:06:34</t>
+          <t>2025-04-11 08:09:05</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-04-22 13:25:34</t>
+          <t>2025-04-11 08:24:05</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-04-22 13:25:34</t>
+          <t>2025-04-11 08:24:05</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-04-23 08:44:12</t>
+          <t>2025-04-16 13:11:46</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>12712</v>
+        <v>122665</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1755,53 +1743,53 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M23" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>250307</v>
+        <v>250856</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="D24" t="n">
-        <v>146.234375</v>
+        <v>309.2244897959184</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-04-23 08:44:12</t>
+          <t>2025-04-10 07:18:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-04-23 09:01:12</t>
+          <t>2025-04-10 09:15:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-04-23 09:01:12</t>
+          <t>2025-04-10 09:15:00</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-04-23 11:27:26</t>
+          <t>2025-04-10 14:24:13</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>9359</v>
+        <v>15152</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1814,7 +1802,7 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M24" t="n">
         <v>70</v>
@@ -1822,41 +1810,41 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251402</v>
+        <v>251134</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="D25" t="n">
-        <v>154.84375</v>
+        <v>89.73469387755102</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-04-23 11:27:26</t>
+          <t>2025-04-10 14:24:13</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-04-23 11:48:26</t>
+          <t>2025-04-11 07:14:13</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-04-23 11:48:26</t>
+          <t>2025-04-11 07:14:13</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-04-23 14:23:16</t>
+          <t>2025-04-11 08:43:57</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>9910</v>
+        <v>4397</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1869,52 +1857,49 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M25" t="n">
         <v>70</v>
-      </c>
-      <c r="N25" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251235</v>
+        <v>244023</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D26" t="n">
-        <v>89.671875</v>
+        <v>20.3469387755102</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-04-23 14:23:16</t>
+          <t>2025-04-11 08:43:57</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-04-23 14:38:16</t>
+          <t>2025-04-11 09:18:57</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-04-23 14:38:16</t>
+          <t>2025-04-11 09:18:57</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-04-24 08:07:57</t>
+          <t>2025-04-11 09:39:18</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>5739</v>
+        <v>997</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1927,49 +1912,52 @@
         </is>
       </c>
       <c r="L26" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M26" t="n">
         <v>70</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251550</v>
+        <v>245413</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="D27" t="n">
-        <v>557.046875</v>
+        <v>102.0408163265306</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-04-24 08:07:57</t>
+          <t>2025-04-11 09:39:18</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-04-24 08:26:57</t>
+          <t>2025-04-11 10:29:18</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-04-24 08:26:57</t>
+          <t>2025-04-11 10:29:18</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-04-25 09:44:00</t>
+          <t>2025-04-11 12:11:20</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>35651</v>
+        <v>5000</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1988,46 +1976,46 @@
         <v>70</v>
       </c>
       <c r="N27" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>250478</v>
+        <v>251033</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D28" t="n">
-        <v>65.375</v>
+        <v>125.4285714285714</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-04-25 09:44:00</t>
+          <t>2025-04-11 12:11:20</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-04-25 10:03:00</t>
+          <t>2025-04-11 12:51:20</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-04-25 10:03:00</t>
+          <t>2025-04-11 12:51:20</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-04-25 11:08:22</t>
+          <t>2025-04-11 14:56:46</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>4184</v>
+        <v>6146</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2040,49 +2028,52 @@
         </is>
       </c>
       <c r="L28" t="n">
+        <v>2</v>
+      </c>
+      <c r="M28" t="n">
+        <v>70</v>
+      </c>
+      <c r="N28" t="n">
         <v>5</v>
-      </c>
-      <c r="M28" t="n">
-        <v>70</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>250855</v>
+        <v>251100</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D29" t="n">
-        <v>443.890625</v>
+        <v>95.12244897959184</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-04-25 11:08:22</t>
+          <t>2025-04-11 14:56:46</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-04-25 11:27:22</t>
+          <t>2025-04-14 07:41:46</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-04-25 11:27:22</t>
+          <t>2025-04-14 07:41:46</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-04-28 10:51:15</t>
+          <t>2025-04-14 09:16:53</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>28409</v>
+        <v>4661</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2095,49 +2086,52 @@
         </is>
       </c>
       <c r="L29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M29" t="n">
         <v>70</v>
+      </c>
+      <c r="N29" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>250635</v>
+        <v>251327</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D30" t="n">
-        <v>146.390625</v>
+        <v>341.7142857142857</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-04-28 10:51:15</t>
+          <t>2025-04-14 09:16:53</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-04-28 11:12:15</t>
+          <t>2025-04-14 09:51:53</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-04-28 11:12:15</t>
+          <t>2025-04-14 09:51:53</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-04-28 13:38:39</t>
+          <t>2025-04-15 07:33:36</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>9369</v>
+        <v>16744</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2146,53 +2140,56 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L30" t="n">
+        <v>4</v>
+      </c>
+      <c r="M30" t="n">
+        <v>70</v>
+      </c>
+      <c r="N30" t="n">
         <v>6</v>
-      </c>
-      <c r="M30" t="n">
-        <v>70</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>250637</v>
+        <v>250966</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D31" t="n">
-        <v>585.578125</v>
+        <v>122.2676056338028</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-04-28 13:38:39</t>
+          <t>2025-04-10 13:25:00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-04-28 13:53:39</t>
+          <t>2025-04-10 14:12:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-04-28 13:53:39</t>
+          <t>2025-04-10 14:12:00</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-04-30 07:39:14</t>
+          <t>2025-04-11 08:14:16</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>37477</v>
+        <v>8681</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2201,11 +2198,11 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L31" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M31" t="n">
         <v>70</v>
@@ -2213,41 +2210,41 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>250780</v>
+        <v>251519</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D32" t="n">
-        <v>408.3125</v>
+        <v>185.5633802816901</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-04-30 07:39:14</t>
+          <t>2025-04-11 08:14:16</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-04-30 08:02:14</t>
+          <t>2025-04-11 08:54:16</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-04-30 08:02:14</t>
+          <t>2025-04-11 08:54:16</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-04-30 14:50:32</t>
+          <t>2025-04-11 11:59:49</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>26132</v>
+        <v>13175</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2256,56 +2253,53 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L32" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M32" t="n">
         <v>70</v>
-      </c>
-      <c r="N32" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>251150</v>
+        <v>251129</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="D33" t="n">
-        <v>709.375</v>
+        <v>101.3098591549296</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-04-30 14:50:32</t>
+          <t>2025-04-11 11:59:49</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-01 07:07:32</t>
+          <t>2025-04-11 12:51:49</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-05-01 07:07:32</t>
+          <t>2025-04-11 12:51:49</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-02 10:56:55</t>
+          <t>2025-04-11 14:33:08</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>45400</v>
+        <v>7193</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -2314,53 +2308,56 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L33" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="M33" t="n">
-        <v>70</v>
+        <v>76</v>
+      </c>
+      <c r="N33" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>243335</v>
+        <v>251204</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="D34" t="n">
-        <v>464.8450704225352</v>
+        <v>107.9295774647887</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-04-10 14:19:00</t>
+          <t>2025-04-11 14:33:08</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-04-10 14:36:00</t>
+          <t>2025-04-14 07:25:08</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-04-10 14:36:00</t>
+          <t>2025-04-14 07:25:08</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-04-11 14:20:50</t>
+          <t>2025-04-14 09:13:04</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>33004</v>
+        <v>7663</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2369,56 +2366,56 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L34" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M34" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N34" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>251166</v>
+        <v>250986</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>34.5</v>
+        <v>205</v>
       </c>
       <c r="D35" t="n">
-        <v>297.0909090909091</v>
+        <v>282.7183098591549</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-04-10 10:41:00</t>
+          <t>2025-04-14 09:13:04</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-04-10 11:15:30</t>
+          <t>2025-04-14 12:38:04</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-04-10 11:15:30</t>
+          <t>2025-04-14 12:38:04</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-04-11 08:12:35</t>
+          <t>2025-04-15 09:20:47</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>16340</v>
+        <v>20073</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -2427,56 +2424,56 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="M35" t="n">
         <v>70</v>
       </c>
       <c r="N35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>251427</v>
+        <v>251109</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>30.5</v>
+        <v>135</v>
       </c>
       <c r="D36" t="n">
-        <v>445.6363636363636</v>
+        <v>266.5915492957747</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-04-11 08:12:35</t>
+          <t>2025-04-15 09:20:47</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-04-11 08:43:05</t>
+          <t>2025-04-15 11:35:47</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-04-11 08:43:05</t>
+          <t>2025-04-15 11:35:47</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-04-14 08:08:43</t>
+          <t>2025-04-16 08:02:22</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>24510</v>
+        <v>18928</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -2485,56 +2482,56 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="M36" t="n">
         <v>70</v>
       </c>
       <c r="N36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>251281</v>
+        <v>251427</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>30.5</v>
+        <v>80</v>
       </c>
       <c r="D37" t="n">
-        <v>297.0909090909091</v>
+        <v>345.2112676056338</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-04-14 08:08:43</t>
+          <t>2025-04-16 08:02:22</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-04-14 08:39:13</t>
+          <t>2025-04-16 09:22:22</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-04-14 08:39:13</t>
+          <t>2025-04-16 09:22:22</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-04-14 13:36:19</t>
+          <t>2025-04-17 07:07:35</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>16340</v>
+        <v>24510</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -2558,41 +2555,41 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>251280</v>
+        <v>251166</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>30.5</v>
+        <v>35</v>
       </c>
       <c r="D38" t="n">
-        <v>346.6</v>
+        <v>230.1408450704225</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-04-14 13:36:19</t>
+          <t>2025-04-17 07:07:35</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-04-14 14:06:49</t>
+          <t>2025-04-17 07:42:35</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-04-14 14:06:49</t>
+          <t>2025-04-17 07:42:35</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-04-15 11:53:25</t>
+          <t>2025-04-17 11:32:43</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>19063</v>
+        <v>16340</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -2616,41 +2613,41 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>251442</v>
+        <v>245623</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>30.5</v>
+        <v>25</v>
       </c>
       <c r="D39" t="n">
-        <v>297.0909090909091</v>
+        <v>382.8840579710145</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-04-15 11:53:25</t>
+          <t>2025-04-10 07:22:00</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-04-15 12:23:55</t>
+          <t>2025-04-10 07:47:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-04-15 12:23:55</t>
+          <t>2025-04-10 07:47:00</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-04-16 09:21:00</t>
+          <t>2025-04-10 14:09:53</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>16340</v>
+        <v>26419</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -2659,56 +2656,53 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M39" t="n">
-        <v>70</v>
-      </c>
-      <c r="N39" t="n">
-        <v>2</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>251285</v>
+        <v>250479</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="D40" t="n">
-        <v>950.344262295082</v>
+        <v>238.6521739130435</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-04-10 14:33:00</t>
+          <t>2025-04-10 14:09:53</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-04-11 08:33:00</t>
+          <t>2025-04-10 14:54:53</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-04-11 08:33:00</t>
+          <t>2025-04-10 14:54:53</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-04-15 08:23:20</t>
+          <t>2025-04-11 10:53:32</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>57971</v>
+        <v>16467</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -2717,11 +2711,11 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L40" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M40" t="n">
         <v>70</v>
@@ -2729,41 +2723,41 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>250497</v>
+        <v>251025</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D41" t="n">
-        <v>267.4647887323944</v>
+        <v>60.39130434782609</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-04-10 10:00:00</t>
+          <t>2025-04-11 10:53:32</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-04-10 10:46:00</t>
+          <t>2025-04-11 11:28:32</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-04-10 10:46:00</t>
+          <t>2025-04-11 11:28:32</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-04-11 07:13:27</t>
+          <t>2025-04-11 12:28:55</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>18990</v>
+        <v>4167</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -2772,53 +2766,56 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M41" t="n">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="N41" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>245089</v>
+        <v>250866</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D42" t="n">
-        <v>1727.676056338028</v>
+        <v>74.14492753623189</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-04-11 07:13:27</t>
+          <t>2025-04-11 12:28:55</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-04-11 07:28:27</t>
+          <t>2025-04-11 13:08:55</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-04-11 07:28:27</t>
+          <t>2025-04-11 13:08:55</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-04-16 12:16:08</t>
+          <t>2025-04-11 14:23:04</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>122665</v>
+        <v>5116</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -2827,53 +2824,56 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M42" t="n">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="N42" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>250986</v>
+        <v>251094</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>212</v>
+        <v>40</v>
       </c>
       <c r="D43" t="n">
-        <v>282.7183098591549</v>
+        <v>195.6086956521739</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-04-10 13:25:00</t>
+          <t>2025-04-11 14:23:04</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-04-11 08:57:00</t>
+          <t>2025-04-14 07:03:04</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-04-11 08:57:00</t>
+          <t>2025-04-14 07:03:04</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-04-11 13:39:43</t>
+          <t>2025-04-14 10:18:40</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>20073</v>
+        <v>13497</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -2882,56 +2882,56 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L43" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="M43" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N43" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>251109</v>
+        <v>251346</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>135</v>
+        <v>50</v>
       </c>
       <c r="D44" t="n">
-        <v>266.5915492957747</v>
+        <v>55.92753623188405</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-04-11 13:39:43</t>
+          <t>2025-04-14 10:18:40</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-04-14 07:54:43</t>
+          <t>2025-04-14 11:08:40</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-04-14 07:54:43</t>
+          <t>2025-04-14 11:08:40</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-04-14 12:21:18</t>
+          <t>2025-04-14 12:04:36</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>18928</v>
+        <v>3859</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -2940,22 +2940,22 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L44" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="M44" t="n">
         <v>70</v>
       </c>
       <c r="N44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>251025</v>
+        <v>251522</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -2963,33 +2963,33 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D45" t="n">
-        <v>60.39130434782609</v>
+        <v>566.6811594202899</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-04-10 07:22:00</t>
+          <t>2025-04-14 12:04:36</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-04-10 07:57:00</t>
+          <t>2025-04-14 12:59:36</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-04-10 07:57:00</t>
+          <t>2025-04-14 12:59:36</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-04-10 08:57:23</t>
+          <t>2025-04-15 14:26:17</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>4167</v>
+        <v>39101</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3002,13 +3002,13 @@
         </is>
       </c>
       <c r="L45" t="n">
+        <v>2</v>
+      </c>
+      <c r="M45" t="n">
+        <v>70</v>
+      </c>
+      <c r="N45" t="n">
         <v>3</v>
-      </c>
-      <c r="M45" t="n">
-        <v>70</v>
-      </c>
-      <c r="N45" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="46">

</xml_diff>

<commit_message>
Cambiato il codice dell'euristico per far sì che effettivamente tutti i tassativi fossero trattati come tali; cambiato il funzionamento del flag in base all'estrazione; semplificato il primo ciclo dell'euristico; ricerche locali funzionano nuovamente, ma escludono e non reincludono più una serie di commesse tassative; rimane da capire perché
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/insert_inter.xlsx
+++ b/PS-VRP/OUTPUT_TEST/insert_inter.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,7 +512,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251561</v>
+        <v>251485</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
         <v>21</v>
       </c>
       <c r="D2" t="n">
-        <v>84.921875</v>
+        <v>75.125</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -542,11 +542,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-07 08:45:55</t>
+          <t>2025-05-07 08:36:07</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>5435</v>
+        <v>4808</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -566,7 +566,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -578,7 +578,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251564</v>
+        <v>251626</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -589,30 +589,30 @@
         <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>42.453125</v>
+        <v>195.3125</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-07 08:45:55</t>
+          <t>2025-05-07 08:36:07</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-07 09:04:55</t>
+          <t>2025-05-07 08:55:07</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-07 09:04:55</t>
+          <t>2025-05-07 08:55:07</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-07 09:47:22</t>
+          <t>2025-05-07 12:10:26</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>2717</v>
+        <v>12500</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -632,7 +632,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O3" t="n">
@@ -644,7 +644,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251566</v>
+        <v>251424</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -655,30 +655,30 @@
         <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>107.640625</v>
+        <v>150.96875</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-07 09:47:22</t>
+          <t>2025-05-07 12:10:26</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:04:22</t>
+          <t>2025-05-07 12:27:26</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:04:22</t>
+          <t>2025-05-07 12:27:26</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-07 11:52:00</t>
+          <t>2025-05-07 14:58:24</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>6889</v>
+        <v>9662</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -710,7 +710,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251519</v>
+        <v>251416</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -721,30 +721,30 @@
         <v>19</v>
       </c>
       <c r="D5" t="n">
-        <v>205.859375</v>
+        <v>175.34375</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-07 11:52:00</t>
+          <t>2025-05-07 14:58:24</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-07 12:11:00</t>
+          <t>2025-05-08 07:17:24</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-07 12:11:00</t>
+          <t>2025-05-08 07:17:24</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-08 07:36:52</t>
+          <t>2025-05-08 10:12:45</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>13175</v>
+        <v>11222</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -762,10 +762,8 @@
       <c r="M5" t="n">
         <v>70</v>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+      <c r="N5" t="n">
+        <v>39755</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
@@ -776,7 +774,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251397</v>
+        <v>251251</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -784,33 +782,33 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D6" t="n">
-        <v>84.921875</v>
+        <v>247.8125</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:36:52</t>
+          <t>2025-05-08 10:12:45</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:53:52</t>
+          <t>2025-05-08 10:35:45</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:53:52</t>
+          <t>2025-05-08 10:35:45</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-08 09:18:47</t>
+          <t>2025-05-08 14:43:33</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>5435</v>
+        <v>15860</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -819,18 +817,18 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M6" t="n">
         <v>70</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O6" t="n">
@@ -842,7 +840,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251475</v>
+        <v>251809</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -850,29 +848,29 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
         <v>135.640625</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-08 09:18:47</t>
+          <t>2025-05-08 14:43:33</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-08 09:35:47</t>
+          <t>2025-05-09 07:02:33</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-08 09:35:47</t>
+          <t>2025-05-09 07:02:33</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-08 11:51:26</t>
+          <t>2025-05-09 09:18:12</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -908,7 +906,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251594</v>
+        <v>251564</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -916,33 +914,33 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>101.03125</v>
+        <v>42.453125</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-08 11:51:26</t>
+          <t>2025-05-09 09:18:12</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:06:26</t>
+          <t>2025-05-09 09:35:12</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:06:26</t>
+          <t>2025-05-09 09:35:12</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-08 13:47:28</t>
+          <t>2025-05-09 10:17:39</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>6466</v>
+        <v>2717</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -955,7 +953,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
@@ -974,7 +972,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>244355</v>
+        <v>251566</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -982,33 +980,33 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>67.34375</v>
+        <v>107.640625</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-08 13:47:28</t>
+          <t>2025-05-09 10:17:39</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 14:02:28</t>
+          <t>2025-05-09 10:34:39</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 14:02:28</t>
+          <t>2025-05-09 10:34:39</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-09 07:09:48</t>
+          <t>2025-05-09 12:22:17</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>4310</v>
+        <v>6889</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1040,7 +1038,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>245623</v>
+        <v>251519</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1048,33 +1046,33 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D10" t="n">
-        <v>412.796875</v>
+        <v>205.859375</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-09 07:09:48</t>
+          <t>2025-05-09 12:22:17</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-09 07:43:48</t>
+          <t>2025-05-09 12:41:17</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-09 07:43:48</t>
+          <t>2025-05-09 12:41:17</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-09 14:36:36</t>
+          <t>2025-05-12 08:07:09</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>26419</v>
+        <v>13175</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1083,14 +1081,14 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
         <v>2</v>
       </c>
       <c r="M10" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1106,7 +1104,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>245089</v>
+        <v>251397</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1114,33 +1112,33 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
-        <v>1916.640625</v>
+        <v>84.921875</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-09 14:36:36</t>
+          <t>2025-05-12 08:07:09</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-12 07:10:36</t>
+          <t>2025-05-12 08:24:09</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-12 07:10:36</t>
+          <t>2025-05-12 08:24:09</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-16 07:07:15</t>
+          <t>2025-05-12 09:49:04</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>122665</v>
+        <v>5435</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1149,14 +1147,14 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1172,37 +1170,37 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251809</v>
+        <v>251475</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D12" t="n">
-        <v>142.3114754098361</v>
+        <v>135.640625</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 09:49:04</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 10:06:04</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 10:06:04</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-09 10:04:18</t>
+          <t>2025-05-12 12:21:43</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1238,41 +1236,41 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251795</v>
+        <v>251594</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D13" t="n">
-        <v>307.1967213114754</v>
+        <v>101.03125</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-09 10:04:18</t>
+          <t>2025-05-12 12:21:43</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-09 10:33:18</t>
+          <t>2025-05-12 12:36:43</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-09 10:33:18</t>
+          <t>2025-05-12 12:36:43</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:30</t>
+          <t>2025-05-12 14:17:45</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>18739</v>
+        <v>6466</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1281,11 +1279,11 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
@@ -1304,41 +1302,41 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>235572</v>
+        <v>244355</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D14" t="n">
-        <v>163.2459016393443</v>
+        <v>67.34375</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:30</t>
+          <t>2025-05-12 14:17:45</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-12 08:07:30</t>
+          <t>2025-05-12 14:32:45</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-12 08:07:30</t>
+          <t>2025-05-12 14:32:45</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-12 10:50:45</t>
+          <t>2025-05-13 07:40:05</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>9958</v>
+        <v>4310</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1347,18 +1345,18 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M14" t="n">
         <v>70</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O14" t="n">
@@ -1370,41 +1368,41 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251259</v>
+        <v>251561</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>81.9672131147541</v>
+        <v>84.921875</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-12 10:50:45</t>
+          <t>2025-05-13 07:40:05</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-12 11:23:45</t>
+          <t>2025-05-13 07:57:05</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-12 11:23:45</t>
+          <t>2025-05-13 07:57:05</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-12 12:45:43</t>
+          <t>2025-05-13 09:22:00</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>5000</v>
+        <v>5435</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1417,14 +1415,14 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O15" t="n">
@@ -1436,41 +1434,41 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>250759</v>
+        <v>251987</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D16" t="n">
-        <v>137.672131147541</v>
+        <v>3289.46875</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-12 12:45:43</t>
+          <t>2025-05-13 09:22:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-12 13:35:43</t>
+          <t>2025-05-13 09:54:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-12 13:35:43</t>
+          <t>2025-05-13 09:54:00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-13 07:53:23</t>
+          <t>2025-05-22 08:43:29</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>8398</v>
+        <v>210526</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1479,11 +1477,11 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M16" t="n">
         <v>76</v>
@@ -1493,18 +1491,16 @@
           <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O16" t="n">
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>39747</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251421</v>
+        <v>250894</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1512,33 +1508,33 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D17" t="n">
-        <v>85.9672131147541</v>
+        <v>725.6065573770492</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-13 07:53:23</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-13 08:20:23</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-13 08:20:23</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-13 09:46:21</t>
+          <t>2025-05-12 11:34:36</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>5244</v>
+        <v>44262</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1547,32 +1543,28 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M17" t="n">
         <v>76</v>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="N17" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>39762</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251463</v>
+        <v>235572</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1580,33 +1572,33 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" t="n">
-        <v>114.2131147540984</v>
+        <v>163.2459016393443</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-13 09:46:21</t>
+          <t>2025-05-12 11:34:36</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-13 10:28:21</t>
+          <t>2025-05-12 12:14:36</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-13 10:28:21</t>
+          <t>2025-05-12 12:14:36</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-13 12:22:34</t>
+          <t>2025-05-12 14:57:51</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>6967</v>
+        <v>9958</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1615,11 +1607,11 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
@@ -1638,7 +1630,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251462</v>
+        <v>251505</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1646,33 +1638,33 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D19" t="n">
-        <v>102.0655737704918</v>
+        <v>233.6885245901639</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-13 12:22:34</t>
+          <t>2025-05-12 14:57:51</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-13 12:51:34</t>
+          <t>2025-05-13 07:22:51</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-13 12:51:34</t>
+          <t>2025-05-13 07:22:51</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-13 14:33:38</t>
+          <t>2025-05-13 11:16:32</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>6226</v>
+        <v>14255</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1685,7 +1677,7 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M19" t="n">
         <v>70</v>
@@ -1704,7 +1696,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251062</v>
+        <v>251846</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1712,33 +1704,33 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" t="n">
-        <v>370.8852459016393</v>
+        <v>186.7540983606557</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-13 14:33:38</t>
+          <t>2025-05-13 11:16:32</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-14 07:06:38</t>
+          <t>2025-05-13 11:47:32</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-14 07:06:38</t>
+          <t>2025-05-13 11:47:32</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-14 13:17:31</t>
+          <t>2025-05-13 14:54:17</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>22624</v>
+        <v>11392</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1747,11 +1739,11 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M20" t="n">
         <v>70</v>
@@ -1770,41 +1762,41 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251340</v>
+        <v>251373</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D21" t="n">
-        <v>461.9718309859155</v>
+        <v>280.2295081967213</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-13 14:54:17</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-08 07:15:00</t>
+          <t>2025-05-14 07:25:17</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-08 07:15:00</t>
+          <t>2025-05-14 07:25:17</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-08 14:56:58</t>
+          <t>2025-05-14 12:05:31</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>32800</v>
+        <v>17094</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1813,14 +1805,14 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M21" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N21" t="inlineStr">
         <is>
@@ -1840,33 +1832,33 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D22" t="n">
-        <v>151.7746478873239</v>
+        <v>176.655737704918</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-08 14:56:58</t>
+          <t>2025-05-14 12:05:31</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:58</t>
+          <t>2025-05-14 12:32:31</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:58</t>
+          <t>2025-05-14 12:32:31</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-09 10:02:44</t>
+          <t>2025-05-15 07:29:10</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -1902,41 +1894,41 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251750</v>
+        <v>251346</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23" t="n">
-        <v>54.80281690140845</v>
+        <v>63.26229508196721</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-09 10:02:44</t>
+          <t>2025-05-15 07:29:10</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-09 10:34:44</t>
+          <t>2025-05-15 08:02:10</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-09 10:34:44</t>
+          <t>2025-05-15 08:02:10</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-09 11:29:32</t>
+          <t>2025-05-15 09:05:26</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>3891</v>
+        <v>3859</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1945,18 +1937,18 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M23" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O23" t="n">
@@ -1968,41 +1960,41 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>245090</v>
+        <v>251259</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D24" t="n">
-        <v>7277.718309859155</v>
+        <v>81.9672131147541</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-09 11:29:32</t>
+          <t>2025-05-15 09:05:26</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-09 12:03:32</t>
+          <t>2025-05-15 09:32:26</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-09 12:03:32</t>
+          <t>2025-05-15 09:32:26</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-30 13:21:16</t>
+          <t>2025-05-15 10:54:24</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>516718</v>
+        <v>5000</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2011,18 +2003,18 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M24" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O24" t="n">
@@ -2034,41 +2026,41 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251416</v>
+        <v>251245</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>30.5</v>
+        <v>31</v>
       </c>
       <c r="D25" t="n">
-        <v>204.0363636363636</v>
+        <v>12.36065573770492</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-15 10:54:24</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:30</t>
+          <t>2025-05-15 11:25:24</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:30</t>
+          <t>2025-05-15 11:25:24</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-09 10:54:32</t>
+          <t>2025-05-15 11:37:46</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>11222</v>
+        <v>754</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2077,17 +2069,19 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M25" t="n">
         <v>70</v>
       </c>
-      <c r="N25" t="n">
-        <v>39755</v>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
       </c>
       <c r="O25" t="n">
         <v>0</v>
@@ -2098,41 +2092,41 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251505</v>
+        <v>251246</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>36.5</v>
+        <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>259.1818181818182</v>
+        <v>196.7540983606557</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-09 10:54:32</t>
+          <t>2025-05-15 11:37:46</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-09 11:31:02</t>
+          <t>2025-05-15 12:02:46</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-09 11:31:02</t>
+          <t>2025-05-15 12:02:46</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:13</t>
+          <t>2025-05-16 07:19:31</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>14255</v>
+        <v>12002</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2141,11 +2135,11 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M26" t="n">
         <v>70</v>
@@ -2164,41 +2158,41 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>250819</v>
+        <v>251463</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>32.5</v>
+        <v>29</v>
       </c>
       <c r="D27" t="n">
-        <v>155.0363636363636</v>
+        <v>114.2131147540984</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:13</t>
+          <t>2025-05-16 07:19:31</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-12 08:22:43</t>
+          <t>2025-05-16 07:48:31</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-12 08:22:43</t>
+          <t>2025-05-16 07:48:31</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-12 10:57:45</t>
+          <t>2025-05-16 09:42:44</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>8527</v>
+        <v>6967</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2211,7 +2205,7 @@
         </is>
       </c>
       <c r="L27" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M27" t="n">
         <v>70</v>
@@ -2230,41 +2224,41 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251761</v>
+        <v>251462</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>34.5</v>
+        <v>29</v>
       </c>
       <c r="D28" t="n">
-        <v>241.4363636363636</v>
+        <v>102.0655737704918</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-12 10:57:45</t>
+          <t>2025-05-16 09:42:44</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-12 11:32:15</t>
+          <t>2025-05-16 10:11:44</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-12 11:32:15</t>
+          <t>2025-05-16 10:11:44</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-13 07:33:41</t>
+          <t>2025-05-16 11:53:48</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>13279</v>
+        <v>6226</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2277,7 +2271,7 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M28" t="n">
         <v>70</v>
@@ -2296,41 +2290,41 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251246</v>
+        <v>251562</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>34.5</v>
+        <v>25</v>
       </c>
       <c r="D29" t="n">
-        <v>218.2181818181818</v>
+        <v>133.4754098360656</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-13 07:33:41</t>
+          <t>2025-05-16 11:53:48</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-13 08:08:11</t>
+          <t>2025-05-16 12:18:48</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-13 08:08:11</t>
+          <t>2025-05-16 12:18:48</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-13 11:46:24</t>
+          <t>2025-05-16 14:32:16</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>12002</v>
+        <v>8142</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2339,11 +2333,11 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M29" t="n">
         <v>70</v>
@@ -2362,41 +2356,41 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251465</v>
+        <v>251580</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>38.5</v>
+        <v>34</v>
       </c>
       <c r="D30" t="n">
-        <v>113.2</v>
+        <v>100.7464788732394</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-13 11:46:24</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-13 12:24:54</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-13 12:24:54</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-13 14:18:06</t>
+          <t>2025-05-08 09:14:44</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>6226</v>
+        <v>7153</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2409,7 +2403,7 @@
         </is>
       </c>
       <c r="L30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M30" t="n">
         <v>70</v>
@@ -2428,41 +2422,41 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>251557</v>
+        <v>251340</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>30.5</v>
+        <v>34</v>
       </c>
       <c r="D31" t="n">
-        <v>121.9090909090909</v>
+        <v>461.9718309859155</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-05-13 14:18:06</t>
+          <t>2025-05-08 09:14:44</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-05-13 14:48:36</t>
+          <t>2025-05-08 09:48:44</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-05-13 14:48:36</t>
+          <t>2025-05-08 09:48:44</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-05-14 08:50:31</t>
+          <t>2025-05-09 09:30:43</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>6705</v>
+        <v>32800</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2471,18 +2465,18 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L31" t="n">
         <v>2</v>
       </c>
       <c r="M31" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O31" t="n">
@@ -2494,41 +2488,41 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>251252</v>
+        <v>251651</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>38.5</v>
+        <v>21</v>
       </c>
       <c r="D32" t="n">
-        <v>274.2363636363636</v>
+        <v>659.5774647887324</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-05-14 08:50:31</t>
+          <t>2025-05-09 09:30:43</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-05-14 09:29:01</t>
+          <t>2025-05-09 09:51:43</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-05-14 09:29:01</t>
+          <t>2025-05-09 09:51:43</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-05-14 14:03:15</t>
+          <t>2025-05-12 12:51:17</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>15083</v>
+        <v>46830</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2537,19 +2531,17 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M32" t="n">
-        <v>70</v>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N32" t="n">
+        <v>39755</v>
       </c>
       <c r="O32" t="n">
         <v>0</v>
@@ -2560,41 +2552,41 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>251373</v>
+        <v>245090</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D33" t="n">
-        <v>280.2295081967213</v>
+        <v>7277.718309859155</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-12 12:51:17</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-12 13:06:17</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-12 13:06:17</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-08 12:15:13</t>
+          <t>2025-06-02 14:24:00</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>17094</v>
+        <v>516718</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -2603,14 +2595,14 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L33" t="n">
         <v>5</v>
       </c>
       <c r="M33" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N33" t="inlineStr">
         <is>
@@ -2626,41 +2618,41 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>244354</v>
+        <v>251761</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D34" t="n">
-        <v>70.65573770491804</v>
+        <v>187.0281690140845</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-05-08 12:15:13</t>
+          <t>2025-06-02 14:24:00</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-05-08 12:40:13</t>
+          <t>2025-06-02 14:56:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-05-08 12:40:13</t>
+          <t>2025-06-02 14:56:00</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-05-08 13:50:53</t>
+          <t>2025-06-03 10:03:02</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>4310</v>
+        <v>13279</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2680,7 +2672,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O34" t="n">
@@ -2692,41 +2684,41 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>244204</v>
+        <v>251283</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35" t="n">
-        <v>56.91803278688525</v>
+        <v>10.61971830985915</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-05-08 13:50:53</t>
+          <t>2025-06-03 10:03:02</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-08 14:10:53</t>
+          <t>2025-06-03 10:22:02</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-05-08 14:10:53</t>
+          <t>2025-06-03 10:22:02</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-05-09 07:07:48</t>
+          <t>2025-06-03 10:32:39</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>3472</v>
+        <v>754</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -2735,18 +2727,18 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M35" t="n">
         <v>70</v>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O35" t="n">
@@ -2758,41 +2750,41 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>251260</v>
+        <v>245350</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D36" t="n">
-        <v>153.5901639344262</v>
+        <v>393.943661971831</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-05-09 07:07:48</t>
+          <t>2025-06-03 10:32:39</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-09 07:37:48</t>
+          <t>2025-06-03 10:55:39</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-05-09 07:37:48</t>
+          <t>2025-06-03 10:55:39</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-09 10:11:23</t>
+          <t>2025-06-04 09:29:36</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>9369</v>
+        <v>27970</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -2801,18 +2793,18 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M36" t="n">
         <v>70</v>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O36" t="n">
@@ -2828,33 +2820,33 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C37" t="n">
         <v>25</v>
       </c>
       <c r="D37" t="n">
-        <v>106</v>
+        <v>91.07042253521126</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-05-09 10:11:23</t>
+          <t>2025-06-04 09:29:36</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-09 10:36:23</t>
+          <t>2025-06-04 09:54:36</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-05-09 10:36:23</t>
+          <t>2025-06-04 09:54:36</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-05-09 12:22:23</t>
+          <t>2025-06-04 11:25:40</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -2890,41 +2882,41 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>251846</v>
+        <v>251464</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>35</v>
+        <v>34.5</v>
       </c>
       <c r="D38" t="n">
-        <v>186.7540983606557</v>
+        <v>130.0545454545455</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-05-09 12:22:23</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-05-09 12:57:23</t>
+          <t>2025-05-09 07:34:30</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-05-09 12:57:23</t>
+          <t>2025-05-09 07:34:30</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-05-12 08:04:08</t>
+          <t>2025-05-09 09:44:33</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>11392</v>
+        <v>7153</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -2937,7 +2929,7 @@
         </is>
       </c>
       <c r="L38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M38" t="n">
         <v>70</v>
@@ -2956,41 +2948,41 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>251485</v>
+        <v>251247</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>35</v>
+        <v>34.5</v>
       </c>
       <c r="D39" t="n">
-        <v>78.81967213114754</v>
+        <v>489.7090909090909</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-05-12 08:04:08</t>
+          <t>2025-05-09 09:44:33</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-05-12 08:39:08</t>
+          <t>2025-05-09 10:19:03</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-05-12 08:39:08</t>
+          <t>2025-05-09 10:19:03</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-05-12 09:57:58</t>
+          <t>2025-05-12 10:28:45</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>4808</v>
+        <v>26934</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -2999,11 +2991,11 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M39" t="n">
         <v>70</v>
@@ -3022,41 +3014,41 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>251346</v>
+        <v>251520</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>35</v>
+        <v>32.5</v>
       </c>
       <c r="D40" t="n">
-        <v>63.26229508196721</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-05-12 09:57:58</t>
+          <t>2025-05-12 10:28:45</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-05-12 10:32:58</t>
+          <t>2025-05-12 11:01:15</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-05-12 10:32:58</t>
+          <t>2025-05-12 11:01:15</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-05-12 11:36:13</t>
+          <t>2025-05-13 07:58:21</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>3859</v>
+        <v>16340</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3065,11 +3057,11 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L40" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M40" t="n">
         <v>70</v>
@@ -3088,41 +3080,41 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>244023</v>
+        <v>251249</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>30</v>
+        <v>32.5</v>
       </c>
       <c r="D41" t="n">
-        <v>16.34426229508197</v>
+        <v>86.50909090909092</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-05-12 11:36:13</t>
+          <t>2025-05-13 07:58:21</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-05-12 12:06:13</t>
+          <t>2025-05-13 08:30:51</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-05-12 12:06:13</t>
+          <t>2025-05-13 08:30:51</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-05-12 12:22:34</t>
+          <t>2025-05-13 09:57:21</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>997</v>
+        <v>4758</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3131,7 +3123,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L41" t="n">
@@ -3154,7 +3146,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>251283</v>
+        <v>251466</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -3162,33 +3154,33 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D42" t="n">
-        <v>12.36065573770492</v>
+        <v>91.26229508196721</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-05-12 12:22:34</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-05-12 12:42:34</t>
+          <t>2025-05-08 07:25:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-05-12 12:42:34</t>
+          <t>2025-05-08 07:25:00</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-05-12 12:54:56</t>
+          <t>2025-05-08 08:56:15</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>754</v>
+        <v>5567</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3197,11 +3189,11 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M42" t="n">
         <v>70</v>
@@ -3220,7 +3212,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>251245</v>
+        <v>244354</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -3228,33 +3220,33 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D43" t="n">
-        <v>12.36065573770492</v>
+        <v>70.65573770491804</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-05-12 12:54:56</t>
+          <t>2025-05-08 08:56:15</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-05-12 13:14:56</t>
+          <t>2025-05-08 09:21:15</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-05-12 13:14:56</t>
+          <t>2025-05-08 09:21:15</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-05-12 13:27:17</t>
+          <t>2025-05-08 10:31:55</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>754</v>
+        <v>4310</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3263,18 +3255,18 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L43" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M43" t="n">
         <v>70</v>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O43" t="n">
@@ -3286,7 +3278,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>251247</v>
+        <v>244204</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -3297,30 +3289,30 @@
         <v>20</v>
       </c>
       <c r="D44" t="n">
-        <v>441.5409836065574</v>
+        <v>56.91803278688525</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-05-12 13:27:17</t>
+          <t>2025-05-08 10:31:55</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-05-12 13:47:17</t>
+          <t>2025-05-08 10:51:55</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-05-12 13:47:17</t>
+          <t>2025-05-08 10:51:55</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-05-13 13:08:50</t>
+          <t>2025-05-08 11:48:50</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>26934</v>
+        <v>3472</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3329,18 +3321,18 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L44" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M44" t="n">
         <v>70</v>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O44" t="n">
@@ -3352,7 +3344,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>251374</v>
+        <v>251795</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -3360,33 +3352,33 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D45" t="n">
-        <v>448.2459016393443</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-05-13 13:08:50</t>
+          <t>2025-05-08 11:48:50</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-05-13 13:33:50</t>
+          <t>2025-05-08 12:18:50</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-05-13 13:33:50</t>
+          <t>2025-05-08 12:18:50</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-05-14 13:02:04</t>
+          <t>2025-05-09 09:26:01</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>27343</v>
+        <v>18739</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3395,18 +3387,18 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M45" t="n">
         <v>70</v>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O45" t="n">
@@ -3418,41 +3410,41 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>251651</v>
+        <v>251260</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D46" t="n">
-        <v>659.5774647887324</v>
+        <v>153.5901639344262</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-09 09:26:01</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:00</t>
+          <t>2025-05-09 09:46:01</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:00</t>
+          <t>2025-05-09 09:46:01</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-05-12 07:20:34</t>
+          <t>2025-05-09 12:19:37</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>46830</v>
+        <v>9369</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3461,17 +3453,19 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L46" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M46" t="n">
-        <v>76</v>
-      </c>
-      <c r="N46" t="n">
-        <v>39755</v>
+        <v>70</v>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
       <c r="O46" t="n">
         <v>0</v>
@@ -3482,41 +3476,41 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>251268</v>
+        <v>250819</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>139.7868852459016</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-05-12 07:20:34</t>
+          <t>2025-05-09 12:19:37</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-05-12 07:37:34</t>
+          <t>2025-05-09 12:39:37</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-05-12 07:37:34</t>
+          <t>2025-05-09 12:39:37</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-05-12 07:37:34</t>
+          <t>2025-05-09 14:59:24</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>8527</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3525,66 +3519,64 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L47" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M47" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N47" t="inlineStr">
         <is>
           <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O47" t="n">
+        <v>0</v>
       </c>
       <c r="P47" t="n">
-        <v>39666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>243569</v>
+        <v>250641</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D48" t="n">
-        <v>36.63380281690141</v>
+        <v>83.8688524590164</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-05-12 07:37:34</t>
+          <t>2025-05-09 14:59:24</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-05-12 07:54:34</t>
+          <t>2025-05-12 07:19:24</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-05-12 07:54:34</t>
+          <t>2025-05-12 07:19:24</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-05-12 08:31:12</t>
+          <t>2025-05-12 08:43:16</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>2601</v>
+        <v>5116</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -3593,14 +3585,14 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L48" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M48" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N48" t="inlineStr">
         <is>
@@ -3616,41 +3608,41 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>250670</v>
+        <v>244023</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D49" t="n">
-        <v>22.01408450704225</v>
+        <v>16.34426229508197</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-05-12 08:31:12</t>
+          <t>2025-05-12 08:43:16</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-05-12 08:48:12</t>
+          <t>2025-05-12 09:03:16</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-05-12 08:48:12</t>
+          <t>2025-05-12 09:03:16</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-05-12 09:10:13</t>
+          <t>2025-05-12 09:19:37</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>1563</v>
+        <v>997</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -3659,14 +3651,14 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L49" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M49" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N49" t="inlineStr">
         <is>
@@ -3682,41 +3674,41 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>243335</v>
+        <v>251061</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D50" t="n">
-        <v>464.8450704225352</v>
+        <v>393.3934426229508</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-05-12 09:10:13</t>
+          <t>2025-05-12 09:19:37</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-05-12 09:40:13</t>
+          <t>2025-05-12 09:39:37</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-05-12 09:40:13</t>
+          <t>2025-05-12 09:39:37</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-05-13 09:25:04</t>
+          <t>2025-05-13 08:13:00</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>33004</v>
+        <v>23997</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -3725,14 +3717,14 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L50" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M50" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N50" t="inlineStr">
         <is>
@@ -3748,41 +3740,41 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>251987</v>
+        <v>251374</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D51" t="n">
-        <v>2965.154929577465</v>
+        <v>448.2459016393443</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-05-13 09:25:04</t>
+          <t>2025-05-13 08:13:00</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-05-13 09:59:04</t>
+          <t>2025-05-13 08:38:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-05-13 09:59:04</t>
+          <t>2025-05-13 08:38:00</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-05-21 11:24:13</t>
+          <t>2025-05-14 08:06:15</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>210526</v>
+        <v>27343</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -3791,14 +3783,14 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L51" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M51" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N51" t="inlineStr">
         <is>
@@ -3814,41 +3806,41 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>251424</v>
+        <v>245089</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D52" t="n">
-        <v>197.1836734693877</v>
+        <v>1727.676056338028</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-05-08 07:45:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-05-08 07:45:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:11</t>
+          <t>2025-05-14 09:06:40</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>9662</v>
+        <v>122665</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -3857,14 +3849,14 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L52" t="n">
         <v>4</v>
       </c>
       <c r="M52" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N52" t="inlineStr">
         <is>
@@ -3880,41 +3872,41 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>250894</v>
+        <v>243569</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D53" t="n">
-        <v>903.3061224489796</v>
+        <v>36.63380281690141</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:11</t>
+          <t>2025-05-14 09:06:40</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-08 11:44:11</t>
+          <t>2025-05-14 09:23:40</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-08 11:44:11</t>
+          <t>2025-05-14 09:23:40</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-05-12 10:47:29</t>
+          <t>2025-05-14 10:00:18</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>44262</v>
+        <v>2601</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -3923,17 +3915,19 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L53" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M53" t="n">
         <v>76</v>
       </c>
-      <c r="N53" t="n">
-        <v>39755</v>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
       </c>
       <c r="O53" t="n">
         <v>0</v>
@@ -3944,41 +3938,41 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>250641</v>
+        <v>250670</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D54" t="n">
-        <v>104.4081632653061</v>
+        <v>22.01408450704225</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-05-12 10:47:29</t>
+          <t>2025-05-14 10:00:18</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-12 11:29:29</t>
+          <t>2025-05-14 10:17:18</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-05-12 11:29:29</t>
+          <t>2025-05-14 10:17:18</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-05-12 13:13:53</t>
+          <t>2025-05-14 10:39:19</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>5116</v>
+        <v>1563</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -3987,14 +3981,14 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L54" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M54" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N54" t="inlineStr">
         <is>
@@ -4010,41 +4004,41 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>251061</v>
+        <v>251750</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D55" t="n">
-        <v>489.734693877551</v>
+        <v>54.80281690140845</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-05-12 13:13:53</t>
+          <t>2025-05-14 10:39:19</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-12 13:48:53</t>
+          <t>2025-05-14 11:11:19</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-05-12 13:48:53</t>
+          <t>2025-05-14 11:11:19</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-05-13 13:58:37</t>
+          <t>2025-05-14 12:06:07</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>23997</v>
+        <v>3891</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -4053,18 +4047,18 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L55" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M55" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O55" t="n">
@@ -4076,41 +4070,41 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>251580</v>
+        <v>245623</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D56" t="n">
-        <v>145.9795918367347</v>
+        <v>372.0985915492957</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-05-13 13:58:37</t>
+          <t>2025-05-14 12:06:07</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-05-13 14:43:37</t>
+          <t>2025-05-14 12:23:07</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-05-13 14:43:37</t>
+          <t>2025-05-14 12:23:07</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-05-14 09:09:36</t>
+          <t>2025-05-15 10:35:13</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>7153</v>
+        <v>26419</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -4119,18 +4113,18 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L56" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M56" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O56" t="n">
@@ -4142,41 +4136,41 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>251249</v>
+        <v>243335</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D57" t="n">
-        <v>97.10204081632654</v>
+        <v>464.8450704225352</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-05-14 09:09:36</t>
+          <t>2025-05-15 10:35:13</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-14 09:54:36</t>
+          <t>2025-05-15 10:54:13</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-05-14 09:54:36</t>
+          <t>2025-05-15 10:54:13</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-05-14 11:31:42</t>
+          <t>2025-05-16 10:39:04</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>4758</v>
+        <v>33004</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -4185,14 +4179,14 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L57" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M57" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N57" t="inlineStr">
         <is>
@@ -4208,41 +4202,41 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>251453</v>
+        <v>251062</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D58" t="n">
-        <v>70.4225352112676</v>
+        <v>461.7142857142857</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2025-05-09 08:52:25</t>
+          <t>2025-05-09 07:36:42</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>5000</v>
+        <v>22624</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -4251,11 +4245,11 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L58" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M58" t="n">
         <v>70</v>
@@ -4265,18 +4259,16 @@
           <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O58" t="n">
+        <v>0</v>
       </c>
       <c r="P58" t="n">
-        <v>39742</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>251626</v>
+        <v>245275</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -4284,33 +4276,33 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="D59" t="n">
-        <v>176.056338028169</v>
+        <v>342.1690140845071</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-05-09 08:52:25</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-05-09 09:27:25</t>
+          <t>2025-05-09 08:37:00</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-05-09 09:27:25</t>
+          <t>2025-05-09 08:37:00</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2025-05-09 12:23:28</t>
+          <t>2025-05-09 14:19:10</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>12500</v>
+        <v>24294</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -4319,11 +4311,11 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;CASON ;R6</t>
         </is>
       </c>
       <c r="L59" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="M59" t="n">
         <v>70</v>
@@ -4342,7 +4334,7 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>245275</v>
+        <v>251109</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -4350,33 +4342,33 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="D60" t="n">
-        <v>342.1690140845071</v>
+        <v>266.5915492957747</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-05-09 12:23:28</t>
+          <t>2025-05-09 14:19:10</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-09 13:53:28</t>
+          <t>2025-05-12 07:04:10</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-05-09 13:53:28</t>
+          <t>2025-05-12 07:04:10</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-05-12 11:35:38</t>
+          <t>2025-05-12 11:30:45</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>24294</v>
+        <v>18928</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4385,11 +4377,11 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;CASON ;R6</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M60" t="n">
         <v>70</v>
@@ -4408,41 +4400,41 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>251109</v>
+        <v>251465</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D61" t="n">
-        <v>266.5915492957747</v>
+        <v>90.23188405797102</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-05-12 11:35:38</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-12 12:20:38</t>
+          <t>2025-05-12 07:35:00</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-05-12 12:20:38</t>
+          <t>2025-05-12 07:35:00</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-05-13 08:47:14</t>
+          <t>2025-05-12 09:05:13</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>18928</v>
+        <v>6226</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -4451,11 +4443,11 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M61" t="n">
         <v>70</v>
@@ -4474,41 +4466,41 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>251456</v>
+        <v>251467</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D62" t="n">
-        <v>126.7464788732394</v>
+        <v>90.23188405797102</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:47:14</t>
+          <t>2025-05-12 09:05:13</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-13 10:27:14</t>
+          <t>2025-05-12 09:30:13</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-05-13 10:27:14</t>
+          <t>2025-05-12 09:30:13</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-05-13 12:33:59</t>
+          <t>2025-05-12 11:00:27</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>8999</v>
+        <v>6226</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -4521,7 +4513,7 @@
         </is>
       </c>
       <c r="L62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M62" t="n">
         <v>70</v>
@@ -4531,52 +4523,50 @@
           <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O62" t="n">
+        <v>0</v>
       </c>
       <c r="P62" t="n">
-        <v>39746</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>251520</v>
+        <v>251557</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D63" t="n">
-        <v>230.1408450704225</v>
+        <v>97.17391304347827</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-05-13 12:33:59</t>
+          <t>2025-05-12 11:00:27</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-13 13:28:59</t>
+          <t>2025-05-12 11:25:27</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-05-13 13:28:59</t>
+          <t>2025-05-12 11:25:27</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-05-14 09:19:07</t>
+          <t>2025-05-12 13:02:38</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>16340</v>
+        <v>6705</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -4585,11 +4575,11 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L63" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M63" t="n">
         <v>70</v>
@@ -4608,7 +4598,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>245350</v>
+        <v>251252</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -4616,33 +4606,33 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D64" t="n">
-        <v>405.3623188405797</v>
+        <v>218.5942028985507</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-12 13:02:38</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-05-12 08:05:00</t>
+          <t>2025-05-12 13:47:38</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-05-12 08:05:00</t>
+          <t>2025-05-12 13:47:38</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>2025-05-12 14:50:21</t>
+          <t>2025-05-13 09:26:13</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>27970</v>
+        <v>15083</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -4651,11 +4641,11 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L64" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M64" t="n">
         <v>70</v>
@@ -4669,472 +4659,6 @@
         <v>0</v>
       </c>
       <c r="P64" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>251225</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>R9</t>
-        </is>
-      </c>
-      <c r="C65" t="n">
-        <v>60</v>
-      </c>
-      <c r="D65" t="n">
-        <v>0</v>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>2025-05-12 14:50:21</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>2025-05-13 07:50:21</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>2025-05-13 07:50:21</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>2025-05-13 07:50:21</t>
-        </is>
-      </c>
-      <c r="I65" t="n">
-        <v>0</v>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
-        </is>
-      </c>
-      <c r="L65" t="n">
-        <v>4</v>
-      </c>
-      <c r="M65" t="n">
-        <v>76</v>
-      </c>
-      <c r="N65" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P65" t="n">
-        <v>39747</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>251227</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>R9</t>
-        </is>
-      </c>
-      <c r="C66" t="n">
-        <v>25</v>
-      </c>
-      <c r="D66" t="n">
-        <v>0</v>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>2025-05-13 07:50:21</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>2025-05-13 08:15:21</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>2025-05-13 08:15:21</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>2025-05-13 08:15:21</t>
-        </is>
-      </c>
-      <c r="I66" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
-        </is>
-      </c>
-      <c r="L66" t="n">
-        <v>4</v>
-      </c>
-      <c r="M66" t="n">
-        <v>76</v>
-      </c>
-      <c r="N66" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P66" t="n">
-        <v>39746</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>251466</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>R9</t>
-        </is>
-      </c>
-      <c r="C67" t="n">
-        <v>35</v>
-      </c>
-      <c r="D67" t="n">
-        <v>80.68115942028986</v>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>2025-05-13 08:15:21</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>2025-05-13 08:50:21</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>2025-05-13 08:50:21</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>2025-05-13 10:11:02</t>
-        </is>
-      </c>
-      <c r="I67" t="n">
-        <v>5567</v>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L67" t="n">
-        <v>3</v>
-      </c>
-      <c r="M67" t="n">
-        <v>70</v>
-      </c>
-      <c r="N67" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O67" t="n">
-        <v>0</v>
-      </c>
-      <c r="P67" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>251464</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>R9</t>
-        </is>
-      </c>
-      <c r="C68" t="n">
-        <v>30</v>
-      </c>
-      <c r="D68" t="n">
-        <v>103.6666666666667</v>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>2025-05-13 10:11:02</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>2025-05-13 10:41:02</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>2025-05-13 10:41:02</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>2025-05-13 12:24:42</t>
-        </is>
-      </c>
-      <c r="I68" t="n">
-        <v>7153</v>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L68" t="n">
-        <v>4</v>
-      </c>
-      <c r="M68" t="n">
-        <v>70</v>
-      </c>
-      <c r="N68" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O68" t="n">
-        <v>0</v>
-      </c>
-      <c r="P68" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>251467</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>R9</t>
-        </is>
-      </c>
-      <c r="C69" t="n">
-        <v>35</v>
-      </c>
-      <c r="D69" t="n">
-        <v>90.23188405797102</v>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>2025-05-13 12:24:42</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>2025-05-13 12:59:42</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>2025-05-13 12:59:42</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>2025-05-13 14:29:56</t>
-        </is>
-      </c>
-      <c r="I69" t="n">
-        <v>6226</v>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L69" t="n">
-        <v>2</v>
-      </c>
-      <c r="M69" t="n">
-        <v>70</v>
-      </c>
-      <c r="N69" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O69" t="n">
-        <v>0</v>
-      </c>
-      <c r="P69" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>251562</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>R9</t>
-        </is>
-      </c>
-      <c r="C70" t="n">
-        <v>25</v>
-      </c>
-      <c r="D70" t="n">
-        <v>118</v>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>2025-05-13 14:29:56</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>2025-05-13 14:54:56</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>2025-05-13 14:54:56</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>2025-05-14 08:52:56</t>
-        </is>
-      </c>
-      <c r="I70" t="n">
-        <v>8142</v>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L70" t="n">
-        <v>2</v>
-      </c>
-      <c r="M70" t="n">
-        <v>70</v>
-      </c>
-      <c r="N70" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O70" t="n">
-        <v>0</v>
-      </c>
-      <c r="P70" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>251251</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>R9</t>
-        </is>
-      </c>
-      <c r="C71" t="n">
-        <v>45</v>
-      </c>
-      <c r="D71" t="n">
-        <v>229.8550724637681</v>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>2025-05-14 08:52:56</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>2025-05-14 09:37:56</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>2025-05-14 09:37:56</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>2025-05-14 13:27:47</t>
-        </is>
-      </c>
-      <c r="I71" t="n">
-        <v>15860</v>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
-        </is>
-      </c>
-      <c r="L71" t="n">
-        <v>6</v>
-      </c>
-      <c r="M71" t="n">
-        <v>70</v>
-      </c>
-      <c r="N71" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O71" t="n">
-        <v>0</v>
-      </c>
-      <c r="P71" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>